<commit_message>
Ajout des sripts pour la gestion des libraire
</commit_message>
<xml_diff>
--- a/data/partenaire_librairies.xlsx
+++ b/data/partenaire_librairies.xlsx
@@ -1,32 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29629"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_EB2923C32D14344B2027D5831EA285CD1118A76B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9AC880D1-E11E-4C5F-98BA-01F43A3AD2CF}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Librairies Partenaires" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Librairies Partenaires"/>
   </sheets>
-  <calcPr calcId="191028"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -528,8 +511,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -540,8 +524,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFffffff"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -553,11 +544,33 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF4472C4"/>
+        <fgColor rgb="FF4472c4"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFc6c6c6"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFc6c6c6"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFc6c6c6"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFc6c6c6"/>
+      </bottom>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -569,23 +582,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+  <cellXfs count="7">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -596,10 +621,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -637,69 +662,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -723,54 +750,53 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
                 <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
+                <a:tint val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
+                <a:tint val="15000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
+                <a:tint val="94000"/>
                 <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
+              <a:shade val="9500"/>
               <a:satMod val="105000"/>
             </a:schemeClr>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -780,7 +806,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -789,7 +815,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -798,7 +824,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -806,10 +832,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -838,7 +864,7 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
+                <a:tint val="20000"/>
                 <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
@@ -851,13 +877,12 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
                 <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
+                <a:tint val="80000"/>
                 <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
@@ -875,25 +900,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="2" max="2" width="31" customWidth="1"/>
-    <col min="3" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="21" customWidth="1"/>
-    <col min="6" max="6" width="33" customWidth="1"/>
-    <col min="7" max="7" width="19" customWidth="1"/>
-    <col min="8" max="8" width="11" customWidth="1"/>
-    <col min="9" max="9" width="18" customWidth="1"/>
-    <col min="10" max="10" width="15" customWidth="1"/>
+    <col min="1" max="1" style="5" width="27.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="31.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="5" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="5" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="5" width="21.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="5" width="33.005" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="5" width="19.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="6" width="11.005" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="5" width="18.005" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="5" width="15.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -915,7 +944,7 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -925,874 +954,647 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
-      <c r="A2" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+      <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="4">
         <v>385000</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
-      <c r="A3" t="s">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+      <c r="A3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="4">
         <v>290000</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
-      <c r="A4" t="s">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+      <c r="A4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="4">
         <v>175000</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
-      <c r="A5" t="s">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+      <c r="A5" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="4">
         <v>220000</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
-      <c r="A6" t="s">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+      <c r="A6" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="4">
         <v>310000</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
-      <c r="A7" t="s">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+      <c r="A7" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="4">
         <v>195000</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
-      <c r="A8" t="s">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+      <c r="A8" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="4">
         <v>145000</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
-      <c r="A9" t="s">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+      <c r="A9" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="4">
         <v>165000</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
-      <c r="A10" t="s">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+      <c r="A10" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="4">
         <v>520000</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" s="3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
-      <c r="A11" t="s">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+      <c r="A11" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="4">
         <v>890000</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
-      <c r="A12" t="s">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+      <c r="A12" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="4">
         <v>1250000</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J12" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
-      <c r="A13" t="s">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+      <c r="A13" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="4">
         <v>680000</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I13" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" s="3" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
-      <c r="A14" t="s">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+      <c r="A14" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="4">
         <v>750000</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I14" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J14" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
-      <c r="A15" t="s">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+      <c r="A15" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="4">
         <v>420000</v>
       </c>
-      <c r="I15" t="s">
+      <c r="I15" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="J15" t="s">
+      <c r="J15" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
-      <c r="A16" t="s">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+      <c r="A16" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="4">
         <v>580000</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I16" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="J16" t="s">
+      <c r="J16" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
-      <c r="A17" t="s">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+      <c r="A17" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="4">
         <v>295000</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I17" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="J17" t="s">
+      <c r="J17" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
-      <c r="A18" t="s">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+      <c r="A18" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G18" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="4">
         <v>410000</v>
       </c>
-      <c r="I18" t="s">
+      <c r="I18" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="J18" t="s">
+      <c r="J18" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
-      <c r="A19" t="s">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
+      <c r="A19" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="4">
         <v>620000</v>
       </c>
-      <c r="I19" t="s">
+      <c r="I19" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J19" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
-      <c r="A20" t="s">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
+      <c r="A20" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G20" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="4">
         <v>340000</v>
       </c>
-      <c r="I20" t="s">
+      <c r="I20" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="J20" t="s">
+      <c r="J20" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
-      <c r="A21" t="s">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
+      <c r="A21" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G21" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="4">
         <v>275000</v>
       </c>
-      <c r="I21" t="s">
+      <c r="I21" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="J21" t="s">
+      <c r="J21" s="3" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C7CE35FF163FC14288CA6216B36E4D02" ma:contentTypeVersion="11" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="e7f0b34a2c6c1d2c96bbc0b355f91eef">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="514a2abc-9483-43de-8cfd-19197a72cec8" xmlns:ns3="e425dd83-799c-4ff9-a9a6-f6a8064637e1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9c366538a0a75c6c1d2973f9081522d3" ns2:_="" ns3:_="">
-    <xsd:import namespace="514a2abc-9483-43de-8cfd-19197a72cec8"/>
-    <xsd:import namespace="e425dd83-799c-4ff9-a9a6-f6a8064637e1"/>
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all>
-                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
-                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
-              </xsd:all>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="514a2abc-9483-43de-8cfd-19197a72cec8" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceSearchProperties" ma:index="10" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="11" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Balises d’images" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="d4b6e4fd-4af2-4f07-b7d1-18266e58562b" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="15" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="16" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="17" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaLengthInSeconds" ma:index="18" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="e425dd83-799c-4ff9-a9a6-f6a8064637e1" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="TaxCatchAll" ma:index="14" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{5186b3eb-60d2-4154-b03c-a4c7679995e8}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="e425dd83-799c-4ff9-a9a6-f6a8064637e1">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Type de contenu"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Titre"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
-    <xs:element name="Person">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:DisplayName" minOccurs="0"/>
-          <xs:element ref="pc:AccountId" minOccurs="0"/>
-          <xs:element ref="pc:AccountType" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="DisplayName" type="xs:string"/>
-    <xs:element name="AccountId" type="xs:string"/>
-    <xs:element name="AccountType" type="xs:string"/>
-    <xs:element name="BDCAssociatedEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-        <xs:attribute ref="pc:EntityNamespace"/>
-        <xs:attribute ref="pc:EntityName"/>
-        <xs:attribute ref="pc:SystemInstanceName"/>
-        <xs:attribute ref="pc:AssociationName"/>
-      </xs:complexType>
-    </xs:element>
-    <xs:attribute name="EntityNamespace" type="xs:string"/>
-    <xs:attribute name="EntityName" type="xs:string"/>
-    <xs:attribute name="SystemInstanceName" type="xs:string"/>
-    <xs:attribute name="AssociationName" type="xs:string"/>
-    <xs:element name="BDCEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
-          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
-          <xs:element ref="pc:EntityId1" minOccurs="0"/>
-          <xs:element ref="pc:EntityId2" minOccurs="0"/>
-          <xs:element ref="pc:EntityId3" minOccurs="0"/>
-          <xs:element ref="pc:EntityId4" minOccurs="0"/>
-          <xs:element ref="pc:EntityId5" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="EntityDisplayName" type="xs:string"/>
-    <xs:element name="EntityInstanceReference" type="xs:string"/>
-    <xs:element name="EntityId1" type="xs:string"/>
-    <xs:element name="EntityId2" type="xs:string"/>
-    <xs:element name="EntityId3" type="xs:string"/>
-    <xs:element name="EntityId4" type="xs:string"/>
-    <xs:element name="EntityId5" type="xs:string"/>
-    <xs:element name="Terms">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermInfo">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermName" minOccurs="0"/>
-          <xs:element ref="pc:TermId" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermName" type="xs:string"/>
-    <xs:element name="TermId" type="xs:string"/>
-  </xs:schema>
-</ct:contentTypeSchema>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="514a2abc-9483-43de-8cfd-19197a72cec8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="e425dd83-799c-4ff9-a9a6-f6a8064637e1" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C69501B-423F-4D3D-903C-74F51980DF14}"/>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{603853AE-F4C7-4017-9C0F-23076AD5D5F7}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E0EE373-A6C6-4D5D-9059-92E98ACF4F58}"/>
 </file>
</xml_diff>